<commit_message>
Documented my project with relevant screenshots
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/ND/ND-2024/RAW_RESULTS/SECOND-YEAR-SECOND-SEMESTER.xlsx
+++ b/EXAMS_INTERNAL/ND/ND-2024/RAW_RESULTS/SECOND-YEAR-SECOND-SEMESTER.xlsx
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5526,8 +5526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6560,7 +6560,7 @@
         <v>14.25714285714286</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>14.714285714285714</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>13.942857142857143</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>16.642857142857142</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>13.542857142857144</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>12.528571428571427</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>12.842857142857145</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>12.328571428571429</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>12.328571428571429</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="16" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9737,8 +9737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11052,7 +11052,7 @@
         <v>53</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="G30" s="1">
         <v>43.5</v>

</xml_diff>